<commit_message>
Attempted optimisation of sigmoid parameters. Need to validate results.
</commit_message>
<xml_diff>
--- a/A fibre ramp positions.xlsx
+++ b/A fibre ramp positions.xlsx
@@ -38,13 +38,13 @@
     <t>End ramp</t>
   </si>
   <si>
-    <t>/home/daniel/Encoding Thermal Stimuli/Matlab files/Exp 19 baseline data.mat</t>
-  </si>
-  <si>
-    <t>/home/daniel/Encoding Thermal Stimuli/Matlab files/Exp 27 unit 1 data.mat</t>
-  </si>
-  <si>
-    <t>/home/daniel/Encoding Thermal Stimuli/Matlab files/Exp 27 unit 2 data.mat</t>
+    <t>/home/daniel/Spike Data/Matlab files/Exp 19 baseline data.mat</t>
+  </si>
+  <si>
+    <t>/home/daniel/Spike Data/Matlab files/Exp 27 unit 1 data.mat</t>
+  </si>
+  <si>
+    <t>/home/daniel/Spike Data/Matlab files/Exp 27 unit 2 data.mat</t>
   </si>
 </sst>
 </file>
@@ -149,7 +149,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Added more C fibre data.
</commit_message>
<xml_diff>
--- a/A fibre ramp positions.xlsx
+++ b/A fibre ramp positions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="76" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="24" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
     <t>End ramp</t>
   </si>
   <si>
-    <t>/home/daniel/Spike Data/Matlab files/Exp 19 baseline data.mat</t>
+    <t>/home/daniel/Spike Data/Matlab files/Exp 19 baseline data new.mat</t>
   </si>
   <si>
     <t>/home/daniel/Spike Data/Matlab files/Exp 27 unit 1 data.mat</t>
@@ -149,7 +149,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -196,28 +196,28 @@
         <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>122700</v>
+        <v>25470</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>124700</v>
+        <v>27430</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>216700</v>
+        <v>119400</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>218400</v>
+        <v>121200</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>296900</v>
+        <v>199600</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>298700</v>
+        <v>201400</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,10 +237,10 @@
         <v>261600</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>399600</v>
+        <v>2976</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>401100</v>
+        <v>5271</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>489400</v>

</xml_diff>

<commit_message>
Added more A fibre data.
</commit_message>
<xml_diff>
--- a/A fibre ramp positions.xlsx
+++ b/A fibre ramp positions.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Full file name</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>/home/daniel/Spike Data/Matlab files/Exp 27 unit 2 data.mat</t>
+  </si>
+  <si>
+    <t>/home/daniel/Spike Data/Matlab files/Exp 6 baseline.mat</t>
+  </si>
+  <si>
+    <t>/home/daniel/Spike Data/Matlab files/exp 30.mat</t>
+  </si>
+  <si>
+    <t>/home/daniel/Spike Data/Matlab files/exp 31.mat</t>
   </si>
 </sst>
 </file>
@@ -146,10 +155,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -278,6 +287,87 @@
         <v>318500</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>10750</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>12800</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>109400</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>111200</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>189600</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>191300</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>16830</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>18330</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>125400</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>127400</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>215100</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>216800</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1424</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2977</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>87050</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>89250</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added resting rate to model.
</commit_message>
<xml_diff>
--- a/A fibre ramp positions.xlsx
+++ b/A fibre ramp positions.xlsx
@@ -15,12 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Full file name</t>
   </si>
   <si>
     <t>Spikes channel num</t>
+  </si>
+  <si>
+    <t>Resting Rate</t>
   </si>
   <si>
     <t>Number of trials</t>
@@ -155,20 +158,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.6683673469388"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1428571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -194,177 +198,198 @@
         <v>6</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>25470</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <v>27430</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="0" t="n">
         <v>119400</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>121200</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>199600</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="J2" s="0" t="n">
         <v>201400</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>259100</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="F3" s="0" t="n">
         <v>261600</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="G3" s="0" t="n">
         <v>2976</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>5271</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>489400</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <v>491500</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>3</v>
+        <v>8.67</v>
       </c>
       <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>77110</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="F4" s="0" t="n">
         <v>79580</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>192500</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>195400</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>315800</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>318500</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>3</v>
+        <v>2.27</v>
       </c>
       <c r="D5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>10750</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="F5" s="0" t="n">
         <v>12800</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="G5" s="0" t="n">
         <v>109400</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <v>111200</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="I5" s="0" t="n">
         <v>189600</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="J5" s="0" t="n">
         <v>191300</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>3</v>
+        <v>6.53</v>
       </c>
       <c r="D6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>16830</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="F6" s="0" t="n">
         <v>18330</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="G6" s="0" t="n">
         <v>125400</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="H6" s="0" t="n">
         <v>127400</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="I6" s="0" t="n">
         <v>215100</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="J6" s="0" t="n">
         <v>216800</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="D7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="0" t="n">
         <v>1424</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="F7" s="0" t="n">
         <v>2977</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>87050</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <v>89250</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Saving before adjusting firing rate in model.
</commit_message>
<xml_diff>
--- a/A fibre ramp positions.xlsx
+++ b/A fibre ramp positions.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Full file name</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>/home/daniel/Spike Data/Matlab files/exp 31.mat</t>
+  </si>
+  <si>
+    <t>old</t>
   </si>
 </sst>
 </file>
@@ -158,10 +161,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -215,7 +218,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>3</v>
@@ -247,7 +250,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>3</v>
@@ -279,7 +282,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>8.67</v>
+        <v>6.5</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3</v>
@@ -311,7 +314,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>2.27</v>
+        <v>7.5</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>3</v>
@@ -343,7 +346,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>6.53</v>
+        <v>3</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>3</v>
@@ -375,7 +378,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0.2</v>
+        <v>8</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2</v>
@@ -391,6 +394,41 @@
       </c>
       <c r="H7" s="0" t="n">
         <v>89250</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H22" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H23" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H24" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H25" s="0" t="n">
+        <v>8.67</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H26" s="0" t="n">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H27" s="0" t="n">
+        <v>6.53</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H28" s="0" t="n">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Grouped response into 'fall','rise' and 'plateau' groups.
</commit_message>
<xml_diff>
--- a/A fibre ramp positions.xlsx
+++ b/A fibre ramp positions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="24" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="8" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Full file name</t>
   </si>
@@ -23,12 +23,12 @@
     <t>Spikes channel num</t>
   </si>
   <si>
+    <t>Number of trials</t>
+  </si>
+  <si>
     <t>Resting Rate</t>
   </si>
   <si>
-    <t>Number of trials</t>
-  </si>
-  <si>
     <t>Start of ramp</t>
   </si>
   <si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>/home/daniel/Spike Data/Matlab files/exp 31.mat</t>
-  </si>
-  <si>
-    <t>old</t>
   </si>
 </sst>
 </file>
@@ -161,19 +158,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.6683673469388"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4744897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.1428571428571"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.0867346938776"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -198,15 +194,21 @@
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -218,10 +220,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>25470</v>
@@ -230,15 +232,21 @@
         <v>27430</v>
       </c>
       <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>119400</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>121200</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="n">
         <v>199600</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="L2" s="0" t="n">
         <v>201400</v>
       </c>
     </row>
@@ -250,10 +258,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>259100</v>
@@ -262,15 +270,21 @@
         <v>261600</v>
       </c>
       <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>2976</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>5271</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="0" t="n">
         <v>489400</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="L3" s="0" t="n">
         <v>491500</v>
       </c>
     </row>
@@ -282,10 +296,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>77110</v>
@@ -294,15 +308,21 @@
         <v>79580</v>
       </c>
       <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="n">
         <v>192500</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>195400</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="0" t="n">
         <v>315800</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="L4" s="0" t="n">
         <v>318500</v>
       </c>
     </row>
@@ -314,10 +334,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>7.5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>10750</v>
@@ -326,15 +346,21 @@
         <v>12800</v>
       </c>
       <c r="G5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
         <v>109400</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="I5" s="0" t="n">
         <v>111200</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
         <v>189600</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="L5" s="0" t="n">
         <v>191300</v>
       </c>
     </row>
@@ -349,7 +375,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>16830</v>
@@ -358,15 +384,21 @@
         <v>18330</v>
       </c>
       <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
         <v>125400</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="I6" s="0" t="n">
         <v>127400</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="n">
         <v>215100</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="L6" s="0" t="n">
         <v>216800</v>
       </c>
     </row>
@@ -378,10 +410,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1424</v>
@@ -390,45 +422,13 @@
         <v>2977</v>
       </c>
       <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>87050</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>89250</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H22" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H23" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H24" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H25" s="0" t="n">
-        <v>8.67</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H26" s="0" t="n">
-        <v>2.27</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H27" s="0" t="n">
-        <v>6.53</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="0" t="n">
-        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a Poisson spike generator to the model.
</commit_message>
<xml_diff>
--- a/A fibre ramp positions.xlsx
+++ b/A fibre ramp positions.xlsx
@@ -161,7 +161,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -299,7 +299,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0</v>
+        <v>6.7</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>77110</v>
@@ -308,7 +308,7 @@
         <v>79580</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>0</v>
+        <v>8.8</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>192500</v>
@@ -317,7 +317,7 @@
         <v>195400</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>315800</v>
@@ -337,7 +337,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>10750</v>
@@ -346,7 +346,7 @@
         <v>12800</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>109400</v>
@@ -355,7 +355,7 @@
         <v>111200</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>189600</v>
@@ -375,7 +375,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>16830</v>
@@ -384,7 +384,7 @@
         <v>18330</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0</v>
+        <v>5.2</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>125400</v>
@@ -393,7 +393,7 @@
         <v>127400</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>0</v>
+        <v>6.4</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>215100</v>
@@ -422,7 +422,7 @@
         <v>2977</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>87050</v>

</xml_diff>

<commit_message>
Removed redundant files and cleaned project.
</commit_message>
<xml_diff>
--- a/A fibre ramp positions.xlsx
+++ b/A fibre ramp positions.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Full file name</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>/home/daniel/Spike Data/Matlab files/exp 31.mat</t>
+  </si>
+  <si>
+    <t>/home/daniel/Spike Data/Matlab files/exp 30 slow baseline with fast ramp.mat</t>
+  </si>
+  <si>
+    <t>/home/daniel/Spike Data/Matlab files/exp 28 baseline.mat</t>
+  </si>
+  <si>
+    <t>/home/daniel/Spike Data/Matlab files/Exp 41 - two neuronal units slow ramps.mat</t>
+  </si>
+  <si>
+    <t>/home/daniel/Spike Data/Matlab files/exp 37 unit 1.mat</t>
   </si>
 </sst>
 </file>
@@ -158,10 +170,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -431,6 +443,86 @@
         <v>89250</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>13330</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>15050</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>170500</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>172000</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>202800</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>204400</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>101500</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>103500</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>